<commit_message>
add initialization method 2
</commit_message>
<xml_diff>
--- a/example_output/LEAGUE A.xlsx
+++ b/example_output/LEAGUE A.xlsx
@@ -76,15 +76,9 @@
     <t>2021-10-28</t>
   </si>
   <si>
-    <t>2021-10-29</t>
-  </si>
-  <si>
     <t>2021-10-30</t>
   </si>
   <si>
-    <t>2021-11-01</t>
-  </si>
-  <si>
     <t>2021-11-02</t>
   </si>
   <si>
@@ -109,6 +103,9 @@
     <t>2021-11-15</t>
   </si>
   <si>
+    <t>2021-11-16</t>
+  </si>
+  <si>
     <t>2021-11-18</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
     <t>2021-12-13</t>
   </si>
   <si>
+    <t>2021-12-14</t>
+  </si>
+  <si>
     <t>2021-12-16</t>
   </si>
   <si>
@@ -163,6 +163,9 @@
     <t>2021-12-23</t>
   </si>
   <si>
+    <t>2021-12-24</t>
+  </si>
+  <si>
     <t>2021-12-25</t>
   </si>
   <si>
@@ -172,9 +175,6 @@
     <t>2021-12-27</t>
   </si>
   <si>
-    <t>2021-12-28</t>
-  </si>
-  <si>
     <t>2021-12-31</t>
   </si>
   <si>
@@ -217,12 +217,15 @@
     <t>2022-01-22</t>
   </si>
   <si>
-    <t>2022-01-27</t>
+    <t>2022-01-25</t>
   </si>
   <si>
     <t>2022-01-28</t>
   </si>
   <si>
+    <t>2022-01-29</t>
+  </si>
+  <si>
     <t>2022-02-03</t>
   </si>
   <si>
@@ -265,15 +268,18 @@
     <t>2022-02-26</t>
   </si>
   <si>
+    <t>2022-02-27</t>
+  </si>
+  <si>
     <t>2022-03-03</t>
   </si>
   <si>
-    <t>2022-03-04</t>
-  </si>
-  <si>
     <t>2022-03-05</t>
   </si>
   <si>
+    <t>2022-03-06</t>
+  </si>
+  <si>
     <t>2022-03-07</t>
   </si>
   <si>
@@ -310,6 +316,9 @@
     <t>2022-03-26</t>
   </si>
   <si>
+    <t>2022-03-27</t>
+  </si>
+  <si>
     <t>2022-03-31</t>
   </si>
   <si>
@@ -325,25 +334,19 @@
     <t>2022-04-04</t>
   </si>
   <si>
-    <t>2022-04-07</t>
-  </si>
-  <si>
     <t>2022-04-08</t>
   </si>
   <si>
     <t>2022-04-09</t>
   </si>
   <si>
-    <t>2022-04-15</t>
-  </si>
-  <si>
     <t>2022-04-16</t>
   </si>
   <si>
     <t>2022-04-17</t>
   </si>
   <si>
-    <t>2022-04-19</t>
+    <t>2022-04-18</t>
   </si>
   <si>
     <t>2022-04-21</t>
@@ -352,15 +355,15 @@
     <t>2022-04-23</t>
   </si>
   <si>
-    <t>2022-04-24</t>
-  </si>
-  <si>
     <t>2022-04-29</t>
   </si>
   <si>
     <t>2022-04-30</t>
   </si>
   <si>
+    <t>2022-05-03</t>
+  </si>
+  <si>
     <t>2022-05-05</t>
   </si>
   <si>
@@ -379,25 +382,19 @@
     <t>2022-05-15</t>
   </si>
   <si>
-    <t>2022-05-17</t>
+    <t>2022-05-19</t>
   </si>
   <si>
     <t>2022-05-21</t>
   </si>
   <si>
-    <t>2022-05-22</t>
-  </si>
-  <si>
     <t>2022-05-27</t>
   </si>
   <si>
-    <t>2022-05-28</t>
-  </si>
-  <si>
-    <t>2022-05-31</t>
-  </si>
-  <si>
-    <t>2022-06-04</t>
+    <t>2022-05-29</t>
+  </si>
+  <si>
+    <t>2022-06-02</t>
   </si>
   <si>
     <t>2022-06-10</t>
@@ -406,24 +403,30 @@
     <t>2022-06-11</t>
   </si>
   <si>
+    <t>2022-06-12</t>
+  </si>
+  <si>
     <t>15u</t>
   </si>
   <si>
+    <t>19u</t>
+  </si>
+  <si>
     <t>22u</t>
   </si>
   <si>
     <t>18u45u</t>
   </si>
   <si>
-    <t>19u</t>
-  </si>
-  <si>
     <t>18u30</t>
   </si>
   <si>
     <t>Camp Nou</t>
   </si>
   <si>
+    <t>Yankee Stadium</t>
+  </si>
+  <si>
     <t>Emirates Stadium</t>
   </si>
   <si>
@@ -433,15 +436,12 @@
     <t>Staples Center</t>
   </si>
   <si>
+    <t>Oracle Arena</t>
+  </si>
+  <si>
     <t>Anfield</t>
   </si>
   <si>
-    <t>Oracle Arena</t>
-  </si>
-  <si>
-    <t>Yankee Stadium</t>
-  </si>
-  <si>
     <t>AT&amp;T Stadium</t>
   </si>
   <si>
@@ -463,6 +463,9 @@
     <t>Stallions</t>
   </si>
   <si>
+    <t>Vipers</t>
+  </si>
+  <si>
     <t>Wolves</t>
   </si>
   <si>
@@ -472,13 +475,10 @@
     <t>Raptors</t>
   </si>
   <si>
+    <t>Cobras</t>
+  </si>
+  <si>
     <t>Eagles</t>
-  </si>
-  <si>
-    <t>Cobras</t>
-  </si>
-  <si>
-    <t>Vipers</t>
   </si>
   <si>
     <t>Falcons</t>
@@ -908,15 +908,15 @@
         <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
         <v>137</v>
@@ -925,15 +925,15 @@
         <v>150</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
         <v>138</v>
@@ -942,41 +942,41 @@
         <v>151</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -993,32 +993,32 @@
         <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
         <v>141</v>
@@ -1027,21 +1027,21 @@
         <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E11" t="s">
         <v>148</v>
@@ -1049,44 +1049,44 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E12" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
         <v>138</v>
@@ -1095,24 +1095,24 @@
         <v>151</v>
       </c>
       <c r="E14" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
         <v>149</v>
-      </c>
-      <c r="E15" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1120,7 +1120,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
         <v>144</v>
@@ -1146,21 +1146,21 @@
         <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E18" t="s">
         <v>156</v>
@@ -1171,30 +1171,30 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
         <v>160</v>
@@ -1202,92 +1202,92 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" t="s">
         <v>148</v>
-      </c>
-      <c r="E21" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>130</v>
@@ -1299,109 +1299,109 @@
         <v>158</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D27" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E28" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E29" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C31" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1409,16 +1409,16 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E33" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1429,13 +1429,13 @@
         <v>130</v>
       </c>
       <c r="C34" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E34" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1443,33 +1443,33 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E35" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C36" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1480,13 +1480,13 @@
         <v>134</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E37" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1497,13 +1497,13 @@
         <v>130</v>
       </c>
       <c r="C38" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1514,47 +1514,47 @@
         <v>130</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
+        <v>159</v>
+      </c>
+      <c r="E39" t="s">
         <v>153</v>
-      </c>
-      <c r="E39" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E41" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1562,16 +1562,16 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E42" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1579,16 +1579,16 @@
         <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E43" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1596,16 +1596,16 @@
         <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D44" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1613,16 +1613,16 @@
         <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E45" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1630,16 +1630,16 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E46" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1647,33 +1647,33 @@
         <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E47" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C48" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E48" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1684,13 +1684,13 @@
         <v>130</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E49" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1701,13 +1701,13 @@
         <v>130</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="E50" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1718,10 +1718,10 @@
         <v>130</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E51" t="s">
         <v>149</v>
@@ -1732,16 +1732,16 @@
         <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E52" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1752,13 +1752,13 @@
         <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D53" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E53" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1766,7 +1766,7 @@
         <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C54" t="s">
         <v>144</v>
@@ -1775,7 +1775,7 @@
         <v>157</v>
       </c>
       <c r="E54" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1792,7 +1792,7 @@
         <v>158</v>
       </c>
       <c r="E55" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1826,7 +1826,7 @@
         <v>153</v>
       </c>
       <c r="E57" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1843,7 +1843,7 @@
         <v>159</v>
       </c>
       <c r="E58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1851,33 +1851,33 @@
         <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E59" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D60" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E60" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1885,16 +1885,16 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E61" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1902,16 +1902,16 @@
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E62" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1919,16 +1919,16 @@
         <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D63" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E63" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1939,13 +1939,13 @@
         <v>130</v>
       </c>
       <c r="C64" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D64" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E64" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1953,7 +1953,7 @@
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C65" t="s">
         <v>144</v>
@@ -1962,7 +1962,7 @@
         <v>157</v>
       </c>
       <c r="E65" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1979,7 +1979,7 @@
         <v>158</v>
       </c>
       <c r="E66" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1996,58 +1996,58 @@
         <v>153</v>
       </c>
       <c r="E67" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D68" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E68" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B69" t="s">
         <v>130</v>
       </c>
       <c r="C69" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E69" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B70" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C70" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D70" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E70" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2075,27 +2075,27 @@
         <v>134</v>
       </c>
       <c r="C72" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D72" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E72" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B73" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D73" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E73" t="s">
         <v>158</v>
@@ -2103,36 +2103,36 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D74" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E74" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B75" t="s">
         <v>132</v>
       </c>
       <c r="C75" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D75" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2149,24 +2149,24 @@
         <v>158</v>
       </c>
       <c r="E76" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C77" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D77" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E77" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2174,16 +2174,16 @@
         <v>63</v>
       </c>
       <c r="B78" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C78" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D78" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E78" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2200,7 +2200,7 @@
         <v>159</v>
       </c>
       <c r="E79" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2217,7 +2217,7 @@
         <v>148</v>
       </c>
       <c r="E80" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2225,72 +2225,72 @@
         <v>66</v>
       </c>
       <c r="B81" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C81" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D81" t="s">
+        <v>150</v>
+      </c>
+      <c r="E81" t="s">
         <v>149</v>
-      </c>
-      <c r="E81" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B82" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C82" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D82" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E82" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B83" t="s">
         <v>130</v>
       </c>
       <c r="C83" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D83" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E83" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B84" t="s">
         <v>130</v>
       </c>
       <c r="C84" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D84" t="s">
+        <v>158</v>
+      </c>
+      <c r="E84" t="s">
         <v>152</v>
-      </c>
-      <c r="E84" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B85" t="s">
         <v>130</v>
@@ -2302,29 +2302,29 @@
         <v>159</v>
       </c>
       <c r="E85" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B86" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C86" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D86" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E86" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B87" t="s">
         <v>131</v>
@@ -2336,29 +2336,29 @@
         <v>149</v>
       </c>
       <c r="E87" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B88" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C88" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D88" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E88" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B89" t="s">
         <v>134</v>
@@ -2370,12 +2370,12 @@
         <v>160</v>
       </c>
       <c r="E89" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B90" t="s">
         <v>130</v>
@@ -2387,32 +2387,32 @@
         <v>156</v>
       </c>
       <c r="E90" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B91" t="s">
         <v>130</v>
       </c>
       <c r="C91" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D91" t="s">
+        <v>152</v>
+      </c>
+      <c r="E91" t="s">
         <v>151</v>
-      </c>
-      <c r="E91" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B92" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C92" t="s">
         <v>144</v>
@@ -2421,80 +2421,80 @@
         <v>157</v>
       </c>
       <c r="E92" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B93" t="s">
         <v>130</v>
       </c>
       <c r="C93" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D93" t="s">
+        <v>153</v>
+      </c>
+      <c r="E93" t="s">
         <v>158</v>
-      </c>
-      <c r="E93" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
         <v>130</v>
       </c>
       <c r="C94" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D94" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E94" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B95" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C95" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D95" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E95" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C96" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D96" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E96" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B97" t="s">
         <v>134</v>
@@ -2506,12 +2506,12 @@
         <v>160</v>
       </c>
       <c r="E97" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B98" t="s">
         <v>130</v>
@@ -2523,174 +2523,174 @@
         <v>156</v>
       </c>
       <c r="E98" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C99" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D99" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E99" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B100" t="s">
         <v>130</v>
       </c>
       <c r="C100" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D100" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E100" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B101" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C101" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D101" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E101" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
         <v>130</v>
       </c>
       <c r="C102" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D102" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E102" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B103" t="s">
         <v>130</v>
       </c>
       <c r="C103" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D103" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E103" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B104" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C104" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D104" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E104" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B105" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C105" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D105" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E105" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B106" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C106" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D106" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E106" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B107" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C107" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D107" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E107" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B108" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C108" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D108" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E108" t="s">
         <v>158</v>
@@ -2698,92 +2698,92 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B109" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C109" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D109" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E109" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B110" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C110" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D110" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E110" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B111" t="s">
         <v>130</v>
       </c>
       <c r="C111" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D111" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E111" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B112" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C112" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D112" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E112" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B113" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C113" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D113" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="E113" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B114" t="s">
         <v>133</v>
@@ -2795,49 +2795,49 @@
         <v>154</v>
       </c>
       <c r="E114" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B115" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C115" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D115" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E115" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B116" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C116" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D116" t="s">
+        <v>156</v>
+      </c>
+      <c r="E116" t="s">
         <v>150</v>
-      </c>
-      <c r="E116" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B117" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C117" t="s">
         <v>138</v>
@@ -2846,106 +2846,106 @@
         <v>151</v>
       </c>
       <c r="E117" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B118" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C118" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D118" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E118" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B119" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C119" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D119" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E119" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B120" t="s">
         <v>130</v>
       </c>
       <c r="C120" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D120" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E120" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B121" t="s">
         <v>130</v>
       </c>
       <c r="C121" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D121" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E121" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B122" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C122" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D122" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E122" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B123" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C123" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D123" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E123" t="s">
         <v>158</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B124" t="s">
         <v>134</v>
@@ -2965,12 +2965,12 @@
         <v>160</v>
       </c>
       <c r="E124" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B125" t="s">
         <v>130</v>
@@ -2982,49 +2982,49 @@
         <v>156</v>
       </c>
       <c r="E125" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B126" t="s">
         <v>130</v>
       </c>
       <c r="C126" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D126" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E126" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B127" t="s">
         <v>130</v>
       </c>
       <c r="C127" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D127" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="E127" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B128" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C128" t="s">
         <v>144</v>
@@ -3033,46 +3033,46 @@
         <v>157</v>
       </c>
       <c r="E128" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B129" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D129" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E129" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B130" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D130" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E130" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B131" t="s">
         <v>134</v>
@@ -3084,21 +3084,21 @@
         <v>160</v>
       </c>
       <c r="E131" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B132" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D132" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E132" t="s">
         <v>153</v>
@@ -3106,41 +3106,41 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C133" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D133" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E133" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B134" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C134" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D134" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E134" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B135" t="s">
         <v>130</v>
@@ -3152,24 +3152,24 @@
         <v>158</v>
       </c>
       <c r="E135" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B136" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C136" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D136" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E136" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3186,21 +3186,21 @@
         <v>148</v>
       </c>
       <c r="E137" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B138" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C138" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D138" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E138" t="s">
         <v>155</v>
@@ -3220,21 +3220,21 @@
         <v>160</v>
       </c>
       <c r="E139" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B140" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C140" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D140" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E140" t="s">
         <v>156</v>
@@ -3242,16 +3242,16 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B141" t="s">
         <v>130</v>
       </c>
       <c r="C141" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D141" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E141" t="s">
         <v>157</v>
@@ -3259,16 +3259,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B142" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C142" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D142" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E142" t="s">
         <v>153</v>
@@ -3276,7 +3276,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B143" t="s">
         <v>130</v>
@@ -3293,7 +3293,7 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B144" t="s">
         <v>130</v>
@@ -3305,7 +3305,7 @@
         <v>148</v>
       </c>
       <c r="E144" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3322,7 +3322,7 @@
         <v>154</v>
       </c>
       <c r="E145" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3330,16 +3330,16 @@
         <v>120</v>
       </c>
       <c r="B146" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C146" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D146" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E146" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3347,16 +3347,16 @@
         <v>120</v>
       </c>
       <c r="B147" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C147" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D147" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E147" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3364,16 +3364,16 @@
         <v>121</v>
       </c>
       <c r="B148" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C148" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D148" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E148" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3384,13 +3384,13 @@
         <v>130</v>
       </c>
       <c r="C149" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D149" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E149" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3398,50 +3398,50 @@
         <v>123</v>
       </c>
       <c r="B150" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C150" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D150" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E150" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B151" t="s">
         <v>130</v>
       </c>
       <c r="C151" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D151" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E151" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B152" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C152" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D152" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E152" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3449,16 +3449,16 @@
         <v>125</v>
       </c>
       <c r="B153" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C153" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D153" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E153" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3466,16 +3466,16 @@
         <v>126</v>
       </c>
       <c r="B154" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C154" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D154" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E154" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3486,13 +3486,13 @@
         <v>130</v>
       </c>
       <c r="C155" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D155" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="E155" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3500,16 +3500,16 @@
         <v>128</v>
       </c>
       <c r="B156" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C156" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D156" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E156" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3517,16 +3517,16 @@
         <v>129</v>
       </c>
       <c r="B157" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C157" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D157" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E157" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>